<commit_message>
tudo pronto mais arquivo de validacao do lisa
</commit_message>
<xml_diff>
--- a/entrada2.xlsx
+++ b/entrada2.xlsx
@@ -59,6 +59,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="11.0"/>
@@ -117,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -130,13 +133,16 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -156,6 +162,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -408,61 +417,61 @@
       <c r="B2" s="4">
         <v>0.0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5">
+      <c r="C2" s="5"/>
+      <c r="D2" s="6">
         <f>COUNT(A2:A1048576)</f>
         <v>7</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="6">
-        <v>144.0</v>
-      </c>
-      <c r="B3" s="6">
-        <v>72.0</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="7">
+        <v>0.144</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0.072</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="6">
-        <v>192.0</v>
-      </c>
-      <c r="B4" s="6">
+      <c r="A4" s="7">
+        <v>0.192</v>
+      </c>
+      <c r="B4" s="7">
         <v>0.0</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="6">
-        <v>288.0</v>
-      </c>
-      <c r="B5" s="6">
-        <v>144.0</v>
+      <c r="A5" s="7">
+        <v>0.288</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.144</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="6">
-        <v>384.0</v>
-      </c>
-      <c r="B6" s="6">
+      <c r="A6" s="7">
+        <v>0.384</v>
+      </c>
+      <c r="B6" s="7">
         <v>0.0</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="6">
-        <v>432.0</v>
-      </c>
-      <c r="B7" s="6">
-        <v>72.0</v>
+      <c r="A7" s="7">
+        <v>0.432</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0.072</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="6">
-        <v>576.0</v>
-      </c>
-      <c r="B8" s="6">
+      <c r="A8" s="7">
+        <v>0.576</v>
+      </c>
+      <c r="B8" s="7">
         <v>0.0</v>
       </c>
     </row>
@@ -1493,171 +1502,171 @@
       <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="8"/>
       <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="8">
+      <c r="A2" s="9">
         <v>1.0</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="9">
         <v>2.0</v>
       </c>
-      <c r="C2" s="9">
-        <v>1.9314E8</v>
-      </c>
-      <c r="D2" s="10">
-        <v>5.25</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="11">
+      <c r="C2" s="10">
+        <v>1.9314E11</v>
+      </c>
+      <c r="D2" s="11">
+        <v>5.25E-6</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="12">
         <f>COUNT(A2:A1048576)</f>
         <v>11</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="8">
+      <c r="A3" s="9">
         <v>2.0</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="13">
         <v>4.0</v>
       </c>
-      <c r="C3" s="9">
-        <v>1.9314E8</v>
-      </c>
-      <c r="D3" s="10">
-        <v>5.25</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+      <c r="C3" s="10">
+        <v>1.9314E11</v>
+      </c>
+      <c r="D3" s="11">
+        <v>5.25E-6</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="6">
+      <c r="A4" s="14">
         <v>4.0</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="14">
         <v>6.0</v>
       </c>
-      <c r="C4" s="9">
-        <v>1.9314E8</v>
-      </c>
-      <c r="D4" s="10">
-        <v>5.25</v>
+      <c r="C4" s="10">
+        <v>1.9314E11</v>
+      </c>
+      <c r="D4" s="11">
+        <v>5.25E-6</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="6">
+      <c r="A5" s="14">
         <v>6.0</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="14">
         <v>7.0</v>
       </c>
-      <c r="C5" s="9">
-        <v>1.9314E8</v>
-      </c>
-      <c r="D5" s="10">
-        <v>5.25</v>
+      <c r="C5" s="10">
+        <v>1.9314E11</v>
+      </c>
+      <c r="D5" s="11">
+        <v>5.25E-6</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="6">
+      <c r="A6" s="14">
         <v>2.0</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="14">
         <v>3.0</v>
       </c>
-      <c r="C6" s="9">
-        <v>1.9314E8</v>
-      </c>
-      <c r="D6" s="10">
-        <v>5.25</v>
+      <c r="C6" s="10">
+        <v>1.9314E11</v>
+      </c>
+      <c r="D6" s="11">
+        <v>5.25E-6</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="6">
+      <c r="A7" s="14">
         <v>3.0</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="14">
         <v>4.0</v>
       </c>
-      <c r="C7" s="9">
-        <v>1.9314E8</v>
-      </c>
-      <c r="D7" s="10">
-        <v>5.25</v>
+      <c r="C7" s="10">
+        <v>1.9314E11</v>
+      </c>
+      <c r="D7" s="11">
+        <v>5.25E-6</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="6">
+      <c r="A8" s="14">
         <v>4.0</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="14">
         <v>5.0</v>
       </c>
-      <c r="C8" s="9">
-        <v>1.9314E8</v>
-      </c>
-      <c r="D8" s="10">
-        <v>5.25</v>
+      <c r="C8" s="10">
+        <v>1.9314E11</v>
+      </c>
+      <c r="D8" s="11">
+        <v>5.25E-6</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="6">
+      <c r="A9" s="14">
         <v>5.0</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="14">
         <v>6.0</v>
       </c>
-      <c r="C9" s="9">
-        <v>1.9314E8</v>
-      </c>
-      <c r="D9" s="10">
-        <v>5.25</v>
+      <c r="C9" s="10">
+        <v>1.9314E11</v>
+      </c>
+      <c r="D9" s="11">
+        <v>5.25E-6</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="6">
+      <c r="A10" s="14">
         <v>1.0</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="14">
         <v>3.0</v>
       </c>
-      <c r="C10" s="9">
-        <v>1.9314E8</v>
-      </c>
-      <c r="D10" s="10">
-        <v>5.25</v>
+      <c r="C10" s="10">
+        <v>1.9314E11</v>
+      </c>
+      <c r="D10" s="11">
+        <v>5.25E-6</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="6">
+      <c r="A11" s="14">
         <v>3.0</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="14">
         <v>5.0</v>
       </c>
-      <c r="C11" s="9">
-        <v>1.9314E8</v>
-      </c>
-      <c r="D11" s="10">
-        <v>5.25</v>
+      <c r="C11" s="10">
+        <v>1.9314E11</v>
+      </c>
+      <c r="D11" s="11">
+        <v>5.25E-6</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="6">
+      <c r="A12" s="14">
         <v>5.0</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="14">
         <v>7.0</v>
       </c>
-      <c r="C12" s="9">
-        <v>1.9314E8</v>
-      </c>
-      <c r="D12" s="10">
-        <v>5.25</v>
+      <c r="C12" s="10">
+        <v>1.9314E11</v>
+      </c>
+      <c r="D12" s="11">
+        <v>5.25E-6</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1"/>
@@ -2686,197 +2695,197 @@
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="6">
+      <c r="A2" s="14">
         <v>2.0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="5">
         <v>1.0</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="14">
         <v>-1300.0</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5">
+      <c r="D2" s="5"/>
+      <c r="E2" s="6">
         <f>COUNT(A2:A1048576)</f>
         <v>6</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="6">
+      <c r="A3" s="14">
         <v>2.0</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="5">
         <v>2.0</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="14">
         <v>-1500.0</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="6">
+      <c r="A4" s="14">
         <v>4.0</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="14">
         <v>1.0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="14">
         <v>-1300.0</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="6">
+      <c r="A5" s="14">
         <v>4.0</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="14">
         <v>2.0</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="14">
         <v>-1500.0</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="6">
+      <c r="A6" s="14">
         <v>6.0</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="14">
         <v>1.0</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="14">
         <v>-1300.0</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="6">
+      <c r="A7" s="14">
         <v>6.0</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="14">
         <v>2.0</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="14">
         <v>-1500.0</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" ht="14.25" customHeight="1"/>
     <row r="25" ht="14.25" customHeight="1"/>
@@ -3890,149 +3899,149 @@
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <v>1.0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="5">
         <v>1.0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5">
+      <c r="C2" s="5"/>
+      <c r="D2" s="6">
         <f>COUNT(A2:A1048576)</f>
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="6">
+      <c r="A3" s="14">
         <v>1.0</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="14">
         <v>2.0</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="6">
+      <c r="A4" s="14">
         <v>7.0</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="5">
         <v>2.0</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" ht="14.25" customHeight="1"/>
     <row r="25" ht="14.25" customHeight="1"/>

</xml_diff>